<commit_message>
Hand soldering made not so hellish
</commit_message>
<xml_diff>
--- a/BOMCPM.xlsx
+++ b/BOMCPM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
   <si>
     <t>Components for 1 board:</t>
   </si>
@@ -131,7 +131,7 @@
     <t>THT, 0805_SMD</t>
   </si>
   <si>
-    <t>https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_1-5KR-1501-1_C114555.html</t>
+    <t>https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount-UniOhm_Uniroyal-Elec-0805W8J0152T5E_C26015.html</t>
   </si>
   <si>
     <t>https://lcsc.com/product-detail/Metal-Film-Resistor-TH_TA-I-Tech-RN16T21501F_C172500.html</t>
@@ -146,7 +146,7 @@
     <t>SOT223_SMD</t>
   </si>
   <si>
-    <t>https://lcsc.com/product-detail/Transistors_DIODES_FZT651TA_FZT651TA_C24098.html</t>
+    <t>https://lcsc.com/product-detail/Others_Nexperia_BCP56-10-115_Nexperia-BCP56-10-115_C192156.html</t>
   </si>
   <si>
     <t>R1, R2</t>
@@ -189,7 +189,7 @@
 </t>
   </si>
   <si>
-    <t>https://lcsc.com/product-detail/Male-Header_Double-row-of-needle1-27mm2-36P_C32369.html</t>
+    <t>https://lcsc.com/product-detail/Male-Header_Shenzhen-Cancome-Headers-Pins-2-3P-2-54mm-Straight-line_C124384.html</t>
   </si>
   <si>
     <t>SW1</t>
@@ -201,7 +201,7 @@
     <t>CandK_6x6mm_Tactile_SMD</t>
   </si>
   <si>
-    <t>https://lcsc.com/product-detail/Tactile-Switches_6-6-5mm-IP66_C128950.html</t>
+    <t>https://lcsc.com/product-detail/Tactile-Switches_6-0mm-6-0mm-4-3mm_C111373.html</t>
   </si>
   <si>
     <t>U1</t>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>1M ohm</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount-UniOhm_Uniroyal-Elec-0805W8F1004T5E_C17514.html</t>
   </si>
   <si>
     <t>https://lcsc.com/product-detail/Metal-Film-Resistor-TH_YAGEO-MFR-12FTE52-1M_C172896.html</t>
@@ -838,10 +841,10 @@
         <v>38</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22">
@@ -852,19 +855,19 @@
         <v>1.0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23">
@@ -875,19 +878,19 @@
         <v>1.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24">
@@ -898,10 +901,10 @@
         <v>2.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>11</v>
@@ -910,7 +913,7 @@
         <v>12</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="208">

</xml_diff>

<commit_message>
Changed the switch so that it doesn't pull the reset line low forever
</commit_message>
<xml_diff>
--- a/BOMCPM.xlsx
+++ b/BOMCPM.xlsx
@@ -210,7 +210,7 @@
     <t xml:space="preserve">CandK_6x6mm_Tactile_SMD</t>
   </si>
   <si>
-    <t xml:space="preserve">https://lcsc.com/product-detail/Tactile-Switches_6-0mm-6-0mm-4-3mm_C111373.html</t>
+    <t xml:space="preserve">https://lcsc.com/product-detail/Tactile-Switches_K2-1187SQ-C4SW_C108649.html</t>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
@@ -509,7 +509,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+      <selection pane="topLeft" activeCell="L27" activeCellId="0" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -842,7 +842,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>13</v>
       </c>
@@ -1077,7 +1077,7 @@
     <hyperlink ref="G14" r:id="rId15" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount-UniOhm_Uniroyal-Elec-0805W8F5760T5E_C17761.html"/>
     <hyperlink ref="Q14" r:id="rId16" display="https://lcsc.com/product-detail/Metal-Film-Resistor-TH_470R-4700-1_C58592.html"/>
     <hyperlink ref="G15" r:id="rId17" display="https://lcsc.com/product-detail/Male-Header_Shenzhen-Cancome-Headers-Pins-2-3P-2-54mm-Straight-line_C124384.html"/>
-    <hyperlink ref="G16" r:id="rId18" display="https://lcsc.com/product-detail/Tactile-Switches_6-0mm-6-0mm-4-3mm_C111373.html"/>
+    <hyperlink ref="G16" r:id="rId18" display="https://lcsc.com/product-detail/Tactile-Switches_K2-1187SQ-C4SW_C108649.html"/>
     <hyperlink ref="G17" r:id="rId19" display="https://lcsc.com/product-detail/ATMEL-AVR_ATMEL_ATMEGA32U4-AU_ATMEGA32U4-AU_C44854.html"/>
     <hyperlink ref="G18" r:id="rId20" display="https://lcsc.com/product-detail/Diodes-ESD_Nexperia_PRTR5V0U2X-215_PRTR5V0U2X-215_C12333.html"/>
     <hyperlink ref="G19" r:id="rId21" display="https://lcsc.com/product-detail/High-Precision-Low-TCR-SMD-Resistors_22R-1-25PPM_C65068.html"/>

</xml_diff>